<commit_message>
Updating stats for FNR and changing names
FNR fert and soil added stats

labels changed
soil N uptake -> N uptake soil
fert N uptake -> N uptake fert
</commit_message>
<xml_diff>
--- a/FNR/soils_15N_maturity.xlsx
+++ b/FNR/soils_15N_maturity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\UC Davis\School Work\Linquist Lab\Data\R stats\Phenols and 15N\Phenols and 15 Analysis\FNR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\15N-and-Phenols-California\FNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="22">
   <si>
     <t>Field</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Topdress</t>
   </si>
   <si>
-    <t>DAS</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>127</t>
-  </si>
-  <si>
     <t>soil_recovery_fert_N</t>
   </si>
   <si>
@@ -82,6 +76,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>total_fertN_recovery_percent</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Maturity</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,10 +418,11 @@
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="29.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,39 +433,42 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1">
         <v>4.9752573315013224</v>
@@ -478,25 +485,30 @@
         <v>34.086732933333337</v>
       </c>
       <c r="I2" s="1">
+        <f>G2+E2</f>
+        <v>15.201277211501324</v>
+      </c>
+      <c r="J2" s="1">
         <f>H2+F2</f>
         <v>50.670924038337745</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2021</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1">
         <v>4.9478451915608472</v>
@@ -513,25 +525,30 @@
         <v>29.535312296666667</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I25" si="2">H3+F3</f>
+        <f t="shared" ref="I3:I25" si="2">G3+E3</f>
+        <v>13.808438880560846</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J25" si="3">H3+F3</f>
         <v>46.028129601869495</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2021</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1">
         <v>4.0149053569662758</v>
@@ -549,24 +566,29 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
+        <v>13.150098294966275</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="3"/>
         <v>43.833660983220916</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>6.2475034654709161</v>
@@ -584,24 +606,29 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
+        <v>17.770226355470918</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
         <v>59.234087851569726</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1">
         <v>6.543928700657573</v>
@@ -619,24 +646,29 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
+        <v>17.885528360657574</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
         <v>59.618427868858575</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2021</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>3.0038430696628957</v>
@@ -654,24 +686,29 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
+        <v>10.621725939662895</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="3"/>
         <v>35.405753132209654</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2021</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
         <v>31.245537105449916</v>
@@ -689,199 +726,229 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
+        <v>89.29621244544991</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
         <v>59.530808296966612</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2021</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>23.497345302560788</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ref="F9:F13" si="3">(E9/150)*100</f>
+        <f t="shared" ref="F9:F13" si="4">(E9/150)*100</f>
         <v>15.664896868373859</v>
       </c>
       <c r="G9" s="1">
         <v>42.529626780000001</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H13" si="4">(G9/150)*100</f>
+        <f t="shared" ref="H9:H13" si="5">(G9/150)*100</f>
         <v>28.353084519999999</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
+        <v>66.026972082560789</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
         <v>44.017981388373855</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2021</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
         <v>24.162327914988069</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.108218609992043</v>
       </c>
       <c r="G10" s="1">
         <v>49.350979819999999</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32.900653213333328</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
+        <v>73.513307734988075</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
         <v>49.008871823325372</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>2021</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1">
         <v>34.027321344731192</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.68488089648746</v>
       </c>
       <c r="G11" s="1">
         <v>56.074809739999999</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37.383206493333333</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
+        <v>90.102131084731184</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="3"/>
         <v>60.068087389820789</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2021</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1">
         <v>39.084725065291671</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.056483376861113</v>
       </c>
       <c r="G12" s="1">
         <v>50.638280809999998</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.758853873333337</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
+        <v>89.723005875291676</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
         <v>59.815337250194446</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2021</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1">
         <v>39.485359128166913</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.323572752111275</v>
       </c>
       <c r="G13" s="1">
         <v>47.325111630000002</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31.550074420000001</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
+        <v>86.810470758166915</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="3"/>
         <v>57.873647172111276</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2021</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1">
         <v>4.1152606310517248</v>
@@ -899,24 +966,29 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
+        <v>11.589987626051725</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="3"/>
         <v>38.633292086839084</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>2022</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1">
         <v>6.7562215283812428</v>
@@ -934,24 +1006,29 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
+        <v>16.461296214381242</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="3"/>
         <v>54.870987381270808</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>2022</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1">
         <v>6.9321329626481267</v>
@@ -969,24 +1046,29 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
+        <v>12.371768930648127</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="3"/>
         <v>41.239229768827087</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2022</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1">
         <v>6.8500823547987588</v>
@@ -1004,24 +1086,29 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
+        <v>18.115713384798759</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
         <v>60.385711282662534</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2022</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1">
         <v>8.0325109054427379</v>
@@ -1039,24 +1126,29 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
+        <v>20.064808295442738</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
         <v>66.882694318142455</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>2022</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1">
         <v>6.2108569229686763</v>
@@ -1074,24 +1166,29 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
+        <v>20.148400272968676</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
         <v>67.161334243228922</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>2022</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E20" s="1">
         <v>46.467123885556994</v>
@@ -1109,186 +1206,216 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
+        <v>85.589312065556996</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
         <v>57.059541377037995</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>2022</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E21" s="1">
         <v>39.663833286997992</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" ref="F21:F25" si="5">(E21/150)*100</f>
+        <f t="shared" ref="F21:F25" si="6">(E21/150)*100</f>
         <v>26.44255552466533</v>
       </c>
       <c r="G21" s="1">
         <v>33.569869429999997</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" ref="H21:H25" si="6">(G21/150)*100</f>
+        <f t="shared" ref="H21:H25" si="7">(G21/150)*100</f>
         <v>22.379912953333331</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
+        <v>73.233702716997982</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="3"/>
         <v>48.822468477998662</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>2022</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E22" s="1">
         <v>33.617028862237568</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.411352574825045</v>
       </c>
       <c r="G22" s="1">
         <v>38.077844089999999</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25.385229393333329</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="2"/>
+        <v>71.694872952237574</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="3"/>
         <v>47.796581968158378</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2022</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E23" s="1">
         <v>24.663502175031532</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.442334783354354</v>
       </c>
       <c r="G23" s="1">
         <v>41.007436480000003</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27.338290986666671</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="2"/>
+        <v>65.670938655031534</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
         <v>43.780625770021025</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>2022</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1">
         <v>44.80674619340806</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29.871164128938705</v>
       </c>
       <c r="G24" s="1">
         <v>44.62649476</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>29.750996506666667</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="2"/>
+        <v>89.43324095340806</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="3"/>
         <v>59.622160635605368</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>2022</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
         <v>11</v>
       </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E25" s="1">
         <v>47.448292576189871</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.63219505079325</v>
       </c>
       <c r="G25" s="1">
         <v>36.288856840000001</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.192571226666669</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="2"/>
+        <v>83.73714941618988</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
         <v>55.824766277459915</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>2022</v>
       </c>
+      <c r="M25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated figures based on reviewer's comments
</commit_message>
<xml_diff>
--- a/FNR/soils_15N_maturity.xlsx
+++ b/FNR/soils_15N_maturity.xlsx
@@ -91,8 +91,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -123,9 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
+      <selection activeCell="M2" sqref="M2:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +425,7 @@
     <col min="10" max="10" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -470,34 +473,36 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1">
-        <v>4.9752573315013224</v>
+      <c r="E2" s="2">
+        <v>4.7911912186879002</v>
       </c>
       <c r="F2" s="1">
         <f>(E2/30)*100</f>
-        <v>16.584191105004408</v>
+        <v>15.970637395626333</v>
       </c>
       <c r="G2" s="1">
-        <v>10.226019880000001</v>
+        <v>10.610846932985739</v>
       </c>
       <c r="H2" s="1">
         <f>(G2/30)*100</f>
-        <v>34.086732933333337</v>
+        <v>35.369489776619126</v>
       </c>
       <c r="I2" s="1">
         <f>G2+E2</f>
-        <v>15.201277211501324</v>
+        <v>15.40203815167364</v>
       </c>
       <c r="J2" s="1">
         <f>H2+F2</f>
-        <v>50.670924038337745</v>
+        <v>51.34012717224546</v>
       </c>
       <c r="K2">
         <v>2021</v>
       </c>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -510,34 +515,36 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1">
-        <v>4.9478451915608472</v>
+      <c r="E3" s="2">
+        <v>4.7647932265003048</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F19" si="0">(E3/30)*100</f>
-        <v>16.492817305202827</v>
+        <v>15.882644088334349</v>
       </c>
       <c r="G3" s="1">
-        <v>8.8605936889999999</v>
+        <v>9.1940368270319652</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H19" si="1">(G3/30)*100</f>
-        <v>29.535312296666667</v>
+        <v>30.646789423439884</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I25" si="2">G3+E3</f>
-        <v>13.808438880560846</v>
+        <v>13.958830053532271</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J25" si="3">H3+F3</f>
-        <v>46.028129601869495</v>
+        <v>46.529433511774229</v>
       </c>
       <c r="K3">
         <v>2021</v>
       </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -550,34 +557,36 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1">
-        <v>4.0149053569662758</v>
+      <c r="E4" s="2">
+        <v>3.8663687139083436</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>13.383017856554252</v>
+        <v>12.887895713027811</v>
       </c>
       <c r="G4" s="1">
-        <v>9.1351929379999994</v>
+        <v>9.4789698342020579</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>30.450643126666666</v>
+        <v>31.596566114006858</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>13.150098294966275</v>
+        <v>13.345338548110401</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>43.833660983220916</v>
+        <v>44.484461827034671</v>
       </c>
       <c r="K4">
         <v>2021</v>
       </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -590,34 +599,36 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1">
-        <v>6.2475034654709161</v>
+      <c r="E5" s="2">
+        <v>6.0163689530113142</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>20.82501155156972</v>
+        <v>20.054563176704381</v>
       </c>
       <c r="G5" s="1">
-        <v>11.522722890000001</v>
+        <v>11.956347652120996</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>38.409076300000002</v>
+        <v>39.854492173736652</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>17.770226355470918</v>
+        <v>17.972716605132312</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>59.234087851569726</v>
+        <v>59.909055350441037</v>
       </c>
       <c r="K5">
         <v>2021</v>
       </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -630,34 +641,36 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1">
-        <v>6.543928700657573</v>
+      <c r="E6" s="2">
+        <v>6.3018275512694348</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>21.813095668858576</v>
+        <v>21.006091837564782</v>
       </c>
       <c r="G6" s="1">
-        <v>11.34159966</v>
+        <v>11.768408370944474</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>37.805332200000002</v>
+        <v>39.228027903148252</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>17.885528360657574</v>
+        <v>18.070235922213911</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>59.618427868858575</v>
+        <v>60.234119740713034</v>
       </c>
       <c r="K6">
         <v>2021</v>
       </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -670,34 +683,36 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1">
-        <v>3.0038430696628957</v>
+      <c r="E7" s="2">
+        <v>2.892711990304726</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>10.012810232209652</v>
+        <v>9.6423733010157537</v>
       </c>
       <c r="G7" s="1">
-        <v>7.6178828699999999</v>
+        <v>7.9045601354051254</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>25.392942899999998</v>
+        <v>26.348533784683752</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>10.621725939662895</v>
+        <v>10.797272125709851</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>35.405753132209654</v>
+        <v>35.990907085699504</v>
       </c>
       <c r="K7">
         <v>2021</v>
       </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -710,34 +725,36 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1">
-        <v>31.245537105449916</v>
+      <c r="E8" s="2">
+        <v>30.08956784103556</v>
       </c>
       <c r="F8" s="1">
         <f>(E8/150)*100</f>
-        <v>20.830358070299944</v>
+        <v>20.059711894023707</v>
       </c>
       <c r="G8" s="1">
-        <v>58.050675339999998</v>
+        <v>60.235246718236311</v>
       </c>
       <c r="H8" s="1">
         <f>(G8/150)*100</f>
-        <v>38.700450226666668</v>
+        <v>40.156831145490877</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>89.29621244544991</v>
+        <v>90.324814559271871</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>59.530808296966612</v>
+        <v>60.216543039514583</v>
       </c>
       <c r="K8">
         <v>2021</v>
       </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -750,34 +767,36 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1">
-        <v>23.497345302560788</v>
+      <c r="E9" s="2">
+        <v>22.62803046654366</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ref="F9:F13" si="4">(E9/150)*100</f>
-        <v>15.664896868373859</v>
+        <v>15.08535364436244</v>
       </c>
       <c r="G9" s="1">
-        <v>42.529626780000001</v>
+        <v>44.130107817365911</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ref="H9:H13" si="5">(G9/150)*100</f>
-        <v>28.353084519999999</v>
+        <v>29.420071878243942</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>66.026972082560789</v>
+        <v>66.758138283909574</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>44.017981388373855</v>
+        <v>44.50542552260638</v>
       </c>
       <c r="K9">
         <v>2021</v>
       </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -790,34 +809,36 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1">
-        <v>24.162327914988069</v>
+      <c r="E10" s="2">
+        <v>23.268411182746796</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="4"/>
-        <v>16.108218609992043</v>
+        <v>15.512274121831195</v>
       </c>
       <c r="G10" s="1">
-        <v>49.350979819999999</v>
+        <v>51.208162991584281</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="5"/>
-        <v>32.900653213333328</v>
+        <v>34.138775327722854</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>73.513307734988075</v>
+        <v>74.476574174331077</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>49.008871823325372</v>
+        <v>49.651049449554051</v>
       </c>
       <c r="K10">
         <v>2021</v>
       </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -830,34 +851,36 @@
       <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1">
-        <v>34.027321344731192</v>
+      <c r="E11" s="2">
+        <v>32.768436356065109</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="4"/>
-        <v>22.68488089648746</v>
+        <v>21.84562423737674</v>
       </c>
       <c r="G11" s="1">
-        <v>56.074809739999999</v>
+        <v>58.1850250485586</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="5"/>
-        <v>37.383206493333333</v>
+        <v>38.790016699039064</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>90.102131084731184</v>
+        <v>90.95346140462371</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>60.068087389820789</v>
+        <v>60.635640936415804</v>
       </c>
       <c r="K11">
         <v>2021</v>
       </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -870,34 +893,36 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1">
-        <v>39.084725065291671</v>
+      <c r="E12" s="2">
+        <v>37.63873485135862</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="4"/>
-        <v>26.056483376861113</v>
+        <v>25.092489900905747</v>
       </c>
       <c r="G12" s="1">
-        <v>50.638280809999998</v>
+        <v>52.543907882010018</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="5"/>
-        <v>33.758853873333337</v>
+        <v>35.029271921340012</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>89.723005875291676</v>
+        <v>90.182642733368638</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>59.815337250194446</v>
+        <v>60.121761822245759</v>
       </c>
       <c r="K12">
         <v>2021</v>
       </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -910,34 +935,36 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1">
-        <v>39.485359128166913</v>
+      <c r="E13" s="2">
+        <v>38.024546936253508</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="4"/>
-        <v>26.323572752111275</v>
+        <v>25.349697957502336</v>
       </c>
       <c r="G13" s="1">
-        <v>47.325111630000002</v>
+        <v>49.10605704479763</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="5"/>
-        <v>31.550074420000001</v>
+        <v>32.73737136319842</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>86.810470758166915</v>
+        <v>87.130603981051138</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>57.873647172111276</v>
+        <v>58.087069320700756</v>
       </c>
       <c r="K13">
         <v>2021</v>
       </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -950,34 +977,36 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1">
-        <v>4.1152606310517248</v>
+      <c r="E14" s="2">
+        <v>3.9630112141671456</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>13.717535436839082</v>
+        <v>13.210037380557152</v>
       </c>
       <c r="G14" s="1">
-        <v>7.4747269950000002</v>
+        <v>7.7560169970800921</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>24.915756650000002</v>
+        <v>25.853389990266972</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>11.589987626051725</v>
+        <v>11.719028211247238</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>38.633292086839084</v>
+        <v>39.063427370824122</v>
       </c>
       <c r="K14">
         <v>2022</v>
       </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -990,34 +1019,36 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1">
-        <v>6.7562215283812428</v>
+      <c r="E15" s="2">
+        <v>6.5062663298507912</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>22.520738427937477</v>
+        <v>21.68755443283597</v>
       </c>
       <c r="G15" s="1">
-        <v>9.7050746859999997</v>
+        <v>10.070297454021794</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>32.350248953333335</v>
+        <v>33.567658180072648</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>16.461296214381242</v>
+        <v>16.576563783872587</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>54.870987381270808</v>
+        <v>55.255212612908622</v>
       </c>
       <c r="K15">
         <v>2022</v>
       </c>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1030,34 +1061,36 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1">
-        <v>6.9321329626481267</v>
+      <c r="E16" s="2">
+        <v>6.6756696919221072</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>23.107109875493755</v>
+        <v>22.252232306407024</v>
       </c>
       <c r="G16" s="1">
-        <v>5.4396359680000002</v>
+        <v>5.6443411320498686</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>18.132119893333336</v>
+        <v>18.814470440166229</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>12.371768930648127</v>
+        <v>12.320010823971977</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>41.239229768827087</v>
+        <v>41.066702746573256</v>
       </c>
       <c r="K16">
         <v>2022</v>
       </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1070,34 +1103,36 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="1">
-        <v>6.8500823547987588</v>
+      <c r="E17" s="2">
+        <v>6.5966546529759169</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>22.833607849329198</v>
+        <v>21.988848843253056</v>
       </c>
       <c r="G17" s="1">
-        <v>11.26563103</v>
+        <v>11.689580877675258</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>37.552103433333336</v>
+        <v>38.965269592250863</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>18.115713384798759</v>
+        <v>18.286235530651176</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>60.385711282662534</v>
+        <v>60.954118435503915</v>
       </c>
       <c r="K17">
         <v>2022</v>
       </c>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1110,34 +1145,36 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="1">
-        <v>8.0325109054427379</v>
+      <c r="E18" s="2">
+        <v>7.7353377222317059</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>26.775036351475794</v>
+        <v>25.784459074105687</v>
       </c>
       <c r="G18" s="1">
-        <v>12.03229739</v>
+        <v>12.48509853550938</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>40.107657966666665</v>
+        <v>41.616995118364599</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>20.064808295442738</v>
+        <v>20.220436257741085</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>66.882694318142455</v>
+        <v>67.401454192470283</v>
       </c>
       <c r="K18">
         <v>2022</v>
       </c>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1150,34 +1187,36 @@
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="1">
-        <v>6.2108569229686763</v>
+      <c r="E19" s="2">
+        <v>5.9810781969894506</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>20.702856409895588</v>
+        <v>19.936927323298168</v>
       </c>
       <c r="G19" s="1">
-        <v>13.93754335</v>
+        <v>14.46204299171999</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>46.458477833333333</v>
+        <v>48.206809972399967</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>20.148400272968676</v>
+        <v>20.443121188709441</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>67.161334243228922</v>
+        <v>68.143737295698131</v>
       </c>
       <c r="K19">
         <v>2022</v>
       </c>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1190,34 +1229,36 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="1">
-        <v>46.467123885556994</v>
+      <c r="E20" s="2">
+        <v>44.748012230149762</v>
       </c>
       <c r="F20" s="1">
         <f>(E20/150)*100</f>
-        <v>30.978082590371329</v>
+        <v>29.832008153433176</v>
       </c>
       <c r="G20" s="1">
-        <v>39.122188180000002</v>
+        <v>40.594439996860473</v>
       </c>
       <c r="H20" s="1">
         <f>(G20/150)*100</f>
-        <v>26.081458786666666</v>
+        <v>27.062959997906983</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>85.589312065556996</v>
+        <v>85.342452227010227</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>57.059541377037995</v>
+        <v>56.894968151340159</v>
       </c>
       <c r="K20">
         <v>2022</v>
       </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1230,34 +1271,36 @@
       <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="1">
-        <v>39.663833286997992</v>
+      <c r="E21" s="2">
+        <v>38.196418211562225</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ref="F21:F25" si="6">(E21/150)*100</f>
-        <v>26.44255552466533</v>
+        <v>25.464278807708151</v>
       </c>
       <c r="G21" s="1">
-        <v>33.569869429999997</v>
+        <v>34.833175582539489</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" ref="H21:H25" si="7">(G21/150)*100</f>
-        <v>22.379912953333331</v>
+        <v>23.222117055026324</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>73.233702716997982</v>
+        <v>73.029593794101714</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>48.822468477998662</v>
+        <v>48.686395862734472</v>
       </c>
       <c r="K21">
         <v>2022</v>
       </c>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1270,34 +1313,36 @@
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1">
-        <v>33.617028862237568</v>
+      <c r="E22" s="2">
+        <v>32.373323177341568</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="6"/>
-        <v>22.411352574825045</v>
+        <v>21.582215451561044</v>
       </c>
       <c r="G22" s="1">
-        <v>38.077844089999999</v>
+        <v>39.510795001228132</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="7"/>
-        <v>25.385229393333329</v>
+        <v>26.340530000818756</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="2"/>
-        <v>71.694872952237574</v>
+        <v>71.884118178569707</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="3"/>
-        <v>47.796581968158378</v>
+        <v>47.9227454523798</v>
       </c>
       <c r="K22">
         <v>2022</v>
       </c>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1310,34 +1355,36 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="1">
-        <v>24.663502175031532</v>
+      <c r="E23" s="2">
+        <v>23.751043849513408</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="6"/>
-        <v>16.442334783354354</v>
+        <v>15.834029233008939</v>
       </c>
       <c r="G23" s="1">
-        <v>41.007436480000003</v>
+        <v>42.550634228085869</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="7"/>
-        <v>27.338290986666671</v>
+        <v>28.367089485390579</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="2"/>
-        <v>65.670938655031534</v>
+        <v>66.301678077599277</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="3"/>
-        <v>43.780625770021025</v>
+        <v>44.20111871839952</v>
       </c>
       <c r="K23">
         <v>2022</v>
       </c>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1350,34 +1397,36 @@
       <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1">
-        <v>44.80674619340806</v>
+      <c r="E24" s="2">
+        <v>43.149062369212878</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="6"/>
-        <v>29.871164128938705</v>
+        <v>28.766041579475253</v>
       </c>
       <c r="G24" s="1">
-        <v>44.62649476</v>
+        <v>46.305885444057992</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="7"/>
-        <v>29.750996506666667</v>
+        <v>30.870590296038664</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="2"/>
-        <v>89.43324095340806</v>
+        <v>89.454947813270877</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="3"/>
-        <v>59.622160635605368</v>
+        <v>59.636631875513913</v>
       </c>
       <c r="K24">
         <v>2022</v>
       </c>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1390,32 +1439,34 @@
       <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="1">
-        <v>47.448292576189871</v>
+      <c r="E25" s="2">
+        <v>45.692881309553371</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="6"/>
-        <v>31.63219505079325</v>
+        <v>30.461920873035581</v>
       </c>
       <c r="G25" s="1">
-        <v>36.288856840000001</v>
+        <v>37.654484321044777</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="7"/>
-        <v>24.192571226666669</v>
+        <v>25.102989547363187</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="2"/>
-        <v>83.73714941618988</v>
+        <v>83.347365630598148</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="3"/>
-        <v>55.824766277459915</v>
+        <v>55.564910420398768</v>
       </c>
       <c r="K25">
         <v>2022</v>
       </c>
-      <c r="M25" s="1"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>